<commit_message>
update to 1.4.1: add default row_split_order and col_split_order
</commit_message>
<xml_diff>
--- a/data/Layout.xlsx
+++ b/data/Layout.xlsx
@@ -8,15 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dingw1/Projects/Github/PyComplexHeatmap/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB78423F-68F6-5442-B0A9-377295F125C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92B59BDB-62B9-B744-A5E8-E58198AB109B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16000" activeTab="3" xr2:uid="{543CC8A9-0D0F-B640-9F26-7173421C5B5A}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16000" xr2:uid="{543CC8A9-0D0F-B640-9F26-7173421C5B5A}"/>
   </bookViews>
   <sheets>
     <sheet name="Layout" sheetId="1" r:id="rId1"/>
     <sheet name="Annotations" sheetId="2" r:id="rId2"/>
     <sheet name="Clustermap" sheetId="3" r:id="rId3"/>
-    <sheet name="comparison" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -39,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Legend</t>
   </si>
@@ -834,180 +833,12 @@
 linecolor</t>
     </r>
   </si>
-  <si>
-    <t>PyComplexHeatmap</t>
-  </si>
-  <si>
-    <t>matplotlib</t>
-  </si>
-  <si>
-    <t>seaborn</t>
-  </si>
-  <si>
-    <t>ComplexHeatmap</t>
-  </si>
-  <si>
-    <t>URL</t>
-  </si>
-  <si>
-    <t>https://github.com/DingWB/PyComplexHeatmap</t>
-  </si>
-  <si>
-    <t>https://github.com/matplotlib/matplotlib</t>
-  </si>
-  <si>
-    <t>https://github.com/mwaskom/seaborn</t>
-  </si>
-  <si>
-    <t>https://github.com/jokergoo/ComplexHeatmap</t>
-  </si>
-  <si>
-    <t>Heatmap Annotations</t>
-  </si>
-  <si>
-    <t>✓</t>
-  </si>
-  <si>
-    <t>×</t>
-  </si>
-  <si>
-    <t>Heatmap Split</t>
-  </si>
-  <si>
-    <t>Row / Columns scale</t>
-  </si>
-  <si>
-    <t>Heatmap Splicing</t>
-  </si>
-  <si>
-    <t>Text Annotations</t>
-  </si>
-  <si>
-    <t>Automatically</t>
-  </si>
-  <si>
-    <t>anno_block</t>
-  </si>
-  <si>
-    <t>Clustering</t>
-  </si>
-  <si>
-    <t>Support Missing Values</t>
-  </si>
-  <si>
-    <t>Plot Legends Separately</t>
-  </si>
-  <si>
-    <t>Version</t>
-  </si>
-  <si>
-    <t>1.3.8</t>
-  </si>
-  <si>
-    <t>2.13.1</t>
-  </si>
-  <si>
-    <t>3.7.1</t>
-  </si>
-  <si>
-    <t>Float Annotated Heatmaps</t>
-  </si>
-  <si>
-    <t>custom function</t>
-  </si>
-  <si>
-    <t>Label Annotations</t>
-  </si>
-  <si>
-    <t>Rasterized</t>
-  </si>
-  <si>
-    <t>Automatically Distributed</t>
-  </si>
-  <si>
-    <t>Manually Distributed</t>
-  </si>
-  <si>
-    <t>Programming Language</t>
-  </si>
-  <si>
-    <t>Python</t>
-  </si>
-  <si>
-    <t>R</t>
-  </si>
-  <si>
-    <t>Support Dot Heatmap</t>
-  </si>
-  <si>
-    <t>Description</t>
-  </si>
-  <si>
-    <t>Scale rows or columns using standard scale or z score</t>
-  </si>
-  <si>
-    <t>Add float values on the top of heatmap cells</t>
-  </si>
-  <si>
-    <t>Combine multiple heatmap vertically or horizontal to generate a joint figure</t>
-  </si>
-  <si>
-    <t>Test version</t>
-  </si>
-  <si>
-    <t>Github link</t>
-  </si>
-  <si>
-    <t>Language</t>
-  </si>
-  <si>
-    <t>Plot dot heatmap using different size, colormap and marker for different categories</t>
-  </si>
-  <si>
-    <t>Rasterize the heatmap to reduce the file size</t>
-  </si>
-  <si>
-    <t>Add labels annotations to show the interested rows or columns and merge the labels of the rows/cols belonging to the same group and distribute them evenly throughout the axis without overlapping</t>
-  </si>
-  <si>
-    <t>Dot Heatmap Annotations</t>
-  </si>
-  <si>
-    <t>Add rows/cols annotations to scatterplot heatmap</t>
-  </si>
-  <si>
-    <t>Add different kinds of annotations, including simple annotation, barplot, boxplot and scatterplot annotations</t>
-  </si>
-  <si>
-    <t>Plot Annotations Separately</t>
-  </si>
-  <si>
-    <t>Plot the figure legends together or separately in another figure</t>
-  </si>
-  <si>
-    <t>Plot the heatmap annotations together or separately in another figure</t>
-  </si>
-  <si>
-    <t>packLegend</t>
-  </si>
-  <si>
-    <t>Clustering rows and columns using different clustering methods and metrics</t>
-  </si>
-  <si>
-    <t>Split rows or columns using int number or given annotations</t>
-  </si>
-  <si>
-    <t>Whether support matrix containing NaN (missing values)</t>
-  </si>
-  <si>
-    <t>Add text on the top of simple annotations</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1080,40 +911,8 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
-    <font>
-      <b/>
-      <sz val="14"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="14"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="12"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="14"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="14"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
   </fonts>
-  <fills count="9">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1144,26 +943,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.14999847407452621"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFAA79"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="22">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -1320,122 +1101,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thick">
-        <color auto="1"/>
-      </top>
-      <bottom style="thick">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="dashDot">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="dashDot">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="dashDot">
-        <color indexed="64"/>
-      </top>
-      <bottom style="dashDot">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="dashDot">
-        <color indexed="64"/>
-      </top>
-      <bottom style="dashDot">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="dashDot">
-        <color indexed="64"/>
-      </right>
-      <top style="dashDot">
-        <color indexed="64"/>
-      </top>
-      <bottom style="dashDot">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="dashDot">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="dashDot">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="dashDot">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="dashDot">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="dashDot">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thick">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="74">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1480,165 +1150,6 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="17" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="17" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="17" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="17" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="15" fillId="7" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="15" fillId="8" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="15" fillId="3" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="15" fillId="4" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="15" fillId="3" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="15" fillId="7" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="15" fillId="8" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="15" fillId="3" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="15" fillId="4" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="15" fillId="8" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1655,8 +1166,7 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1979,8 +1489,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44EFBB7E-10ED-0A41-80A6-61F98CFBF3E2}">
   <dimension ref="B1:E5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2001,7 +1511,7 @@
         <v>1</v>
       </c>
       <c r="D2" s="5"/>
-      <c r="E2" s="69" t="s">
+      <c r="E2" s="16" t="s">
         <v>0</v>
       </c>
     </row>
@@ -2015,7 +1525,7 @@
       <c r="D3" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="70"/>
+      <c r="E3" s="17"/>
     </row>
     <row r="4" spans="2:5" ht="53" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B4" s="3"/>
@@ -2023,7 +1533,7 @@
         <v>3</v>
       </c>
       <c r="D4" s="4"/>
-      <c r="E4" s="71"/>
+      <c r="E4" s="18"/>
     </row>
     <row r="5" spans="2:5" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
   </sheetData>
@@ -2090,7 +1600,7 @@
   <dimension ref="A1:A6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20" x14ac:dyDescent="0.2"/>
@@ -2106,21 +1616,21 @@
       </c>
     </row>
     <row r="2" spans="1:1" ht="235" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="72" t="s">
+      <c r="A2" s="19" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="73"/>
+      <c r="A3" s="20"/>
     </row>
     <row r="4" spans="1:1" ht="312" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="73"/>
+      <c r="A4" s="20"/>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A5" s="73"/>
+      <c r="A5" s="20"/>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A6" s="73"/>
+      <c r="A6" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2128,394 +1638,4 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{940C07AC-F826-B94A-B413-2A7A2FCA7B44}">
-  <dimension ref="A1:F19"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="18.5" style="19" customWidth="1"/>
-    <col min="2" max="2" width="23.83203125" style="16" customWidth="1"/>
-    <col min="3" max="3" width="19.33203125" style="16" customWidth="1"/>
-    <col min="4" max="4" width="17.1640625" style="16" customWidth="1"/>
-    <col min="5" max="5" width="21.33203125" style="16" customWidth="1"/>
-    <col min="6" max="6" width="33.6640625" style="19" customWidth="1"/>
-    <col min="7" max="16384" width="10.83203125" style="16"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="20"/>
-      <c r="B1" s="22" t="s">
-        <v>16</v>
-      </c>
-      <c r="C1" s="23" t="s">
-        <v>17</v>
-      </c>
-      <c r="D1" s="24" t="s">
-        <v>18</v>
-      </c>
-      <c r="E1" s="21" t="s">
-        <v>19</v>
-      </c>
-      <c r="F1" s="68" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="20" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="25" t="s">
-        <v>37</v>
-      </c>
-      <c r="B2" s="26" t="s">
-        <v>38</v>
-      </c>
-      <c r="C2" s="27" t="s">
-        <v>40</v>
-      </c>
-      <c r="D2" s="28">
-        <v>0.12</v>
-      </c>
-      <c r="E2" s="29" t="s">
-        <v>39</v>
-      </c>
-      <c r="F2" s="30" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="51" x14ac:dyDescent="0.2">
-      <c r="A3" s="31" t="s">
-        <v>20</v>
-      </c>
-      <c r="B3" s="32" t="s">
-        <v>21</v>
-      </c>
-      <c r="C3" s="33" t="s">
-        <v>22</v>
-      </c>
-      <c r="D3" s="34" t="s">
-        <v>23</v>
-      </c>
-      <c r="E3" s="35" t="s">
-        <v>24</v>
-      </c>
-      <c r="F3" s="36" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" s="18" customFormat="1" ht="19" x14ac:dyDescent="0.2">
-      <c r="A4" s="37" t="s">
-        <v>57</v>
-      </c>
-      <c r="B4" s="38" t="s">
-        <v>48</v>
-      </c>
-      <c r="C4" s="39" t="s">
-        <v>48</v>
-      </c>
-      <c r="D4" s="40" t="s">
-        <v>48</v>
-      </c>
-      <c r="E4" s="41" t="s">
-        <v>49</v>
-      </c>
-      <c r="F4" s="42" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" s="17" customFormat="1" ht="38" x14ac:dyDescent="0.2">
-      <c r="A5" s="43" t="s">
-        <v>29</v>
-      </c>
-      <c r="B5" s="44" t="s">
-        <v>26</v>
-      </c>
-      <c r="C5" s="45" t="s">
-        <v>27</v>
-      </c>
-      <c r="D5" s="46" t="s">
-        <v>26</v>
-      </c>
-      <c r="E5" s="47" t="s">
-        <v>27</v>
-      </c>
-      <c r="F5" s="48" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" s="17" customFormat="1" ht="57" x14ac:dyDescent="0.2">
-      <c r="A6" s="37" t="s">
-        <v>34</v>
-      </c>
-      <c r="B6" s="38" t="s">
-        <v>26</v>
-      </c>
-      <c r="C6" s="39" t="s">
-        <v>27</v>
-      </c>
-      <c r="D6" s="40" t="s">
-        <v>26</v>
-      </c>
-      <c r="E6" s="41" t="s">
-        <v>26</v>
-      </c>
-      <c r="F6" s="42" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" s="17" customFormat="1" ht="57" x14ac:dyDescent="0.2">
-      <c r="A7" s="43" t="s">
-        <v>28</v>
-      </c>
-      <c r="B7" s="44" t="s">
-        <v>26</v>
-      </c>
-      <c r="C7" s="45" t="s">
-        <v>27</v>
-      </c>
-      <c r="D7" s="46" t="s">
-        <v>27</v>
-      </c>
-      <c r="E7" s="47" t="s">
-        <v>26</v>
-      </c>
-      <c r="F7" s="48" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" s="17" customFormat="1" ht="57" x14ac:dyDescent="0.2">
-      <c r="A8" s="37" t="s">
-        <v>35</v>
-      </c>
-      <c r="B8" s="38" t="s">
-        <v>26</v>
-      </c>
-      <c r="C8" s="39" t="s">
-        <v>27</v>
-      </c>
-      <c r="D8" s="40" t="s">
-        <v>27</v>
-      </c>
-      <c r="E8" s="41" t="s">
-        <v>26</v>
-      </c>
-      <c r="F8" s="42" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" s="17" customFormat="1" ht="76" x14ac:dyDescent="0.2">
-      <c r="A9" s="43" t="s">
-        <v>25</v>
-      </c>
-      <c r="B9" s="44" t="s">
-        <v>26</v>
-      </c>
-      <c r="C9" s="45" t="s">
-        <v>27</v>
-      </c>
-      <c r="D9" s="49" t="s">
-        <v>42</v>
-      </c>
-      <c r="E9" s="47" t="s">
-        <v>26</v>
-      </c>
-      <c r="F9" s="48" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" s="17" customFormat="1" ht="38" x14ac:dyDescent="0.2">
-      <c r="A10" s="56" t="s">
-        <v>31</v>
-      </c>
-      <c r="B10" s="38" t="s">
-        <v>32</v>
-      </c>
-      <c r="C10" s="39" t="s">
-        <v>27</v>
-      </c>
-      <c r="D10" s="40" t="s">
-        <v>27</v>
-      </c>
-      <c r="E10" s="41" t="s">
-        <v>33</v>
-      </c>
-      <c r="F10" s="57" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" s="17" customFormat="1" ht="57" x14ac:dyDescent="0.2">
-      <c r="A11" s="50" t="s">
-        <v>41</v>
-      </c>
-      <c r="B11" s="51" t="s">
-        <v>26</v>
-      </c>
-      <c r="C11" s="52" t="s">
-        <v>42</v>
-      </c>
-      <c r="D11" s="53" t="s">
-        <v>26</v>
-      </c>
-      <c r="E11" s="54" t="s">
-        <v>42</v>
-      </c>
-      <c r="F11" s="55" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" s="17" customFormat="1" ht="57" x14ac:dyDescent="0.2">
-      <c r="A12" s="37" t="s">
-        <v>30</v>
-      </c>
-      <c r="B12" s="38" t="s">
-        <v>26</v>
-      </c>
-      <c r="C12" s="39" t="s">
-        <v>27</v>
-      </c>
-      <c r="D12" s="40" t="s">
-        <v>27</v>
-      </c>
-      <c r="E12" s="41" t="s">
-        <v>26</v>
-      </c>
-      <c r="F12" s="42" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" s="17" customFormat="1" ht="76" x14ac:dyDescent="0.2">
-      <c r="A13" s="43" t="s">
-        <v>50</v>
-      </c>
-      <c r="B13" s="44" t="s">
-        <v>26</v>
-      </c>
-      <c r="C13" s="45" t="s">
-        <v>27</v>
-      </c>
-      <c r="D13" s="46" t="s">
-        <v>26</v>
-      </c>
-      <c r="E13" s="47" t="s">
-        <v>42</v>
-      </c>
-      <c r="F13" s="48" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" s="17" customFormat="1" ht="38" x14ac:dyDescent="0.2">
-      <c r="A14" s="37" t="s">
-        <v>61</v>
-      </c>
-      <c r="B14" s="38" t="s">
-        <v>26</v>
-      </c>
-      <c r="C14" s="39" t="s">
-        <v>27</v>
-      </c>
-      <c r="D14" s="58" t="s">
-        <v>42</v>
-      </c>
-      <c r="E14" s="41" t="s">
-        <v>26</v>
-      </c>
-      <c r="F14" s="42" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" s="18" customFormat="1" ht="57" x14ac:dyDescent="0.2">
-      <c r="A15" s="59" t="s">
-        <v>36</v>
-      </c>
-      <c r="B15" s="44" t="s">
-        <v>26</v>
-      </c>
-      <c r="C15" s="45" t="s">
-        <v>27</v>
-      </c>
-      <c r="D15" s="46" t="s">
-        <v>27</v>
-      </c>
-      <c r="E15" s="47" t="s">
-        <v>67</v>
-      </c>
-      <c r="F15" s="60" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" s="18" customFormat="1" ht="57" x14ac:dyDescent="0.2">
-      <c r="A16" s="37" t="s">
-        <v>64</v>
-      </c>
-      <c r="B16" s="38" t="s">
-        <v>26</v>
-      </c>
-      <c r="C16" s="39" t="s">
-        <v>27</v>
-      </c>
-      <c r="D16" s="40" t="s">
-        <v>27</v>
-      </c>
-      <c r="E16" s="41" t="s">
-        <v>26</v>
-      </c>
-      <c r="F16" s="42" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" s="18" customFormat="1" ht="38" x14ac:dyDescent="0.2">
-      <c r="A17" s="59" t="s">
-        <v>44</v>
-      </c>
-      <c r="B17" s="44" t="s">
-        <v>26</v>
-      </c>
-      <c r="C17" s="61" t="s">
-        <v>42</v>
-      </c>
-      <c r="D17" s="46" t="s">
-        <v>26</v>
-      </c>
-      <c r="E17" s="47" t="s">
-        <v>26</v>
-      </c>
-      <c r="F17" s="60" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" s="18" customFormat="1" ht="134" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="62" t="s">
-        <v>43</v>
-      </c>
-      <c r="B18" s="63" t="s">
-        <v>45</v>
-      </c>
-      <c r="C18" s="64" t="s">
-        <v>27</v>
-      </c>
-      <c r="D18" s="65" t="s">
-        <v>27</v>
-      </c>
-      <c r="E18" s="66" t="s">
-        <v>46</v>
-      </c>
-      <c r="F18" s="67" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="19" thickTop="1" x14ac:dyDescent="0.2"/>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B3" r:id="rId1" xr:uid="{978A4675-3171-6E4C-A699-F26B876D2562}"/>
-    <hyperlink ref="C3" r:id="rId2" xr:uid="{B9A34BBA-19FF-F441-B57E-59973E7104DB}"/>
-    <hyperlink ref="D3" r:id="rId3" xr:uid="{B6FCF39D-FA13-1E43-B5EB-36AB35444E04}"/>
-    <hyperlink ref="E3" r:id="rId4" xr:uid="{5FD034E2-35A2-9643-BAAC-F776F2A0A3AB}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
update default vmax,vmin for legend_kws and add default pdf.fonttype
</commit_message>
<xml_diff>
--- a/data/Layout.xlsx
+++ b/data/Layout.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dingw1/Projects/Github/PyComplexHeatmap/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92B59BDB-62B9-B744-A5E8-E58198AB109B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB78423F-68F6-5442-B0A9-377295F125C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16000" xr2:uid="{543CC8A9-0D0F-B640-9F26-7173421C5B5A}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16000" activeTab="3" xr2:uid="{543CC8A9-0D0F-B640-9F26-7173421C5B5A}"/>
   </bookViews>
   <sheets>
     <sheet name="Layout" sheetId="1" r:id="rId1"/>
     <sheet name="Annotations" sheetId="2" r:id="rId2"/>
     <sheet name="Clustermap" sheetId="3" r:id="rId3"/>
+    <sheet name="comparison" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="72">
   <si>
     <t>Legend</t>
   </si>
@@ -833,12 +834,180 @@
 linecolor</t>
     </r>
   </si>
+  <si>
+    <t>PyComplexHeatmap</t>
+  </si>
+  <si>
+    <t>matplotlib</t>
+  </si>
+  <si>
+    <t>seaborn</t>
+  </si>
+  <si>
+    <t>ComplexHeatmap</t>
+  </si>
+  <si>
+    <t>URL</t>
+  </si>
+  <si>
+    <t>https://github.com/DingWB/PyComplexHeatmap</t>
+  </si>
+  <si>
+    <t>https://github.com/matplotlib/matplotlib</t>
+  </si>
+  <si>
+    <t>https://github.com/mwaskom/seaborn</t>
+  </si>
+  <si>
+    <t>https://github.com/jokergoo/ComplexHeatmap</t>
+  </si>
+  <si>
+    <t>Heatmap Annotations</t>
+  </si>
+  <si>
+    <t>✓</t>
+  </si>
+  <si>
+    <t>×</t>
+  </si>
+  <si>
+    <t>Heatmap Split</t>
+  </si>
+  <si>
+    <t>Row / Columns scale</t>
+  </si>
+  <si>
+    <t>Heatmap Splicing</t>
+  </si>
+  <si>
+    <t>Text Annotations</t>
+  </si>
+  <si>
+    <t>Automatically</t>
+  </si>
+  <si>
+    <t>anno_block</t>
+  </si>
+  <si>
+    <t>Clustering</t>
+  </si>
+  <si>
+    <t>Support Missing Values</t>
+  </si>
+  <si>
+    <t>Plot Legends Separately</t>
+  </si>
+  <si>
+    <t>Version</t>
+  </si>
+  <si>
+    <t>1.3.8</t>
+  </si>
+  <si>
+    <t>2.13.1</t>
+  </si>
+  <si>
+    <t>3.7.1</t>
+  </si>
+  <si>
+    <t>Float Annotated Heatmaps</t>
+  </si>
+  <si>
+    <t>custom function</t>
+  </si>
+  <si>
+    <t>Label Annotations</t>
+  </si>
+  <si>
+    <t>Rasterized</t>
+  </si>
+  <si>
+    <t>Automatically Distributed</t>
+  </si>
+  <si>
+    <t>Manually Distributed</t>
+  </si>
+  <si>
+    <t>Programming Language</t>
+  </si>
+  <si>
+    <t>Python</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>Support Dot Heatmap</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Scale rows or columns using standard scale or z score</t>
+  </si>
+  <si>
+    <t>Add float values on the top of heatmap cells</t>
+  </si>
+  <si>
+    <t>Combine multiple heatmap vertically or horizontal to generate a joint figure</t>
+  </si>
+  <si>
+    <t>Test version</t>
+  </si>
+  <si>
+    <t>Github link</t>
+  </si>
+  <si>
+    <t>Language</t>
+  </si>
+  <si>
+    <t>Plot dot heatmap using different size, colormap and marker for different categories</t>
+  </si>
+  <si>
+    <t>Rasterize the heatmap to reduce the file size</t>
+  </si>
+  <si>
+    <t>Add labels annotations to show the interested rows or columns and merge the labels of the rows/cols belonging to the same group and distribute them evenly throughout the axis without overlapping</t>
+  </si>
+  <si>
+    <t>Dot Heatmap Annotations</t>
+  </si>
+  <si>
+    <t>Add rows/cols annotations to scatterplot heatmap</t>
+  </si>
+  <si>
+    <t>Add different kinds of annotations, including simple annotation, barplot, boxplot and scatterplot annotations</t>
+  </si>
+  <si>
+    <t>Plot Annotations Separately</t>
+  </si>
+  <si>
+    <t>Plot the figure legends together or separately in another figure</t>
+  </si>
+  <si>
+    <t>Plot the heatmap annotations together or separately in another figure</t>
+  </si>
+  <si>
+    <t>packLegend</t>
+  </si>
+  <si>
+    <t>Clustering rows and columns using different clustering methods and metrics</t>
+  </si>
+  <si>
+    <t>Split rows or columns using int number or given annotations</t>
+  </si>
+  <si>
+    <t>Whether support matrix containing NaN (missing values)</t>
+  </si>
+  <si>
+    <t>Add text on the top of simple annotations</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -911,8 +1080,40 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -943,8 +1144,26 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFAA79"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="14">
+  <borders count="22">
     <border>
       <left/>
       <right/>
@@ -1101,11 +1320,122 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="dashDot">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dashDot">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="dashDot">
+        <color indexed="64"/>
+      </top>
+      <bottom style="dashDot">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="dashDot">
+        <color indexed="64"/>
+      </top>
+      <bottom style="dashDot">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="dashDot">
+        <color indexed="64"/>
+      </right>
+      <top style="dashDot">
+        <color indexed="64"/>
+      </top>
+      <bottom style="dashDot">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dashDot">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="dashDot">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="dashDot">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="dashDot">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="dashDot">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="74">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1150,6 +1480,165 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="17" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="17" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="17" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="17" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="15" fillId="7" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="15" fillId="8" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="15" fillId="3" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="15" fillId="4" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="15" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="15" fillId="3" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="15" fillId="7" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="15" fillId="8" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="15" fillId="3" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="15" fillId="4" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="15" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="15" fillId="8" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1166,7 +1655,8 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1489,8 +1979,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44EFBB7E-10ED-0A41-80A6-61F98CFBF3E2}">
   <dimension ref="B1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1511,7 +2001,7 @@
         <v>1</v>
       </c>
       <c r="D2" s="5"/>
-      <c r="E2" s="16" t="s">
+      <c r="E2" s="69" t="s">
         <v>0</v>
       </c>
     </row>
@@ -1525,7 +2015,7 @@
       <c r="D3" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="17"/>
+      <c r="E3" s="70"/>
     </row>
     <row r="4" spans="2:5" ht="53" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B4" s="3"/>
@@ -1533,7 +2023,7 @@
         <v>3</v>
       </c>
       <c r="D4" s="4"/>
-      <c r="E4" s="18"/>
+      <c r="E4" s="71"/>
     </row>
     <row r="5" spans="2:5" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
   </sheetData>
@@ -1600,7 +2090,7 @@
   <dimension ref="A1:A6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20" x14ac:dyDescent="0.2"/>
@@ -1616,21 +2106,21 @@
       </c>
     </row>
     <row r="2" spans="1:1" ht="235" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="72" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="20"/>
+      <c r="A3" s="73"/>
     </row>
     <row r="4" spans="1:1" ht="312" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="20"/>
+      <c r="A4" s="73"/>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A5" s="20"/>
+      <c r="A5" s="73"/>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A6" s="20"/>
+      <c r="A6" s="73"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1638,4 +2128,394 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{940C07AC-F826-B94A-B413-2A7A2FCA7B44}">
+  <dimension ref="A1:F19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="18.5" style="19" customWidth="1"/>
+    <col min="2" max="2" width="23.83203125" style="16" customWidth="1"/>
+    <col min="3" max="3" width="19.33203125" style="16" customWidth="1"/>
+    <col min="4" max="4" width="17.1640625" style="16" customWidth="1"/>
+    <col min="5" max="5" width="21.33203125" style="16" customWidth="1"/>
+    <col min="6" max="6" width="33.6640625" style="19" customWidth="1"/>
+    <col min="7" max="16384" width="10.83203125" style="16"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="20"/>
+      <c r="B1" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="F1" s="68" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="20" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="25" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2" s="27" t="s">
+        <v>40</v>
+      </c>
+      <c r="D2" s="28">
+        <v>0.12</v>
+      </c>
+      <c r="E2" s="29" t="s">
+        <v>39</v>
+      </c>
+      <c r="F2" s="30" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+      <c r="A3" s="31" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="32" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" s="33" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="34" t="s">
+        <v>23</v>
+      </c>
+      <c r="E3" s="35" t="s">
+        <v>24</v>
+      </c>
+      <c r="F3" s="36" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" s="18" customFormat="1" ht="19" x14ac:dyDescent="0.2">
+      <c r="A4" s="37" t="s">
+        <v>57</v>
+      </c>
+      <c r="B4" s="38" t="s">
+        <v>48</v>
+      </c>
+      <c r="C4" s="39" t="s">
+        <v>48</v>
+      </c>
+      <c r="D4" s="40" t="s">
+        <v>48</v>
+      </c>
+      <c r="E4" s="41" t="s">
+        <v>49</v>
+      </c>
+      <c r="F4" s="42" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" s="17" customFormat="1" ht="38" x14ac:dyDescent="0.2">
+      <c r="A5" s="43" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5" s="44" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" s="45" t="s">
+        <v>27</v>
+      </c>
+      <c r="D5" s="46" t="s">
+        <v>26</v>
+      </c>
+      <c r="E5" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="F5" s="48" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" s="17" customFormat="1" ht="57" x14ac:dyDescent="0.2">
+      <c r="A6" s="37" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6" s="38" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" s="39" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6" s="40" t="s">
+        <v>26</v>
+      </c>
+      <c r="E6" s="41" t="s">
+        <v>26</v>
+      </c>
+      <c r="F6" s="42" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" s="17" customFormat="1" ht="57" x14ac:dyDescent="0.2">
+      <c r="A7" s="43" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7" s="44" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" s="45" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" s="46" t="s">
+        <v>27</v>
+      </c>
+      <c r="E7" s="47" t="s">
+        <v>26</v>
+      </c>
+      <c r="F7" s="48" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" s="17" customFormat="1" ht="57" x14ac:dyDescent="0.2">
+      <c r="A8" s="37" t="s">
+        <v>35</v>
+      </c>
+      <c r="B8" s="38" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8" s="39" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" s="40" t="s">
+        <v>27</v>
+      </c>
+      <c r="E8" s="41" t="s">
+        <v>26</v>
+      </c>
+      <c r="F8" s="42" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" s="17" customFormat="1" ht="76" x14ac:dyDescent="0.2">
+      <c r="A9" s="43" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" s="44" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" s="45" t="s">
+        <v>27</v>
+      </c>
+      <c r="D9" s="49" t="s">
+        <v>42</v>
+      </c>
+      <c r="E9" s="47" t="s">
+        <v>26</v>
+      </c>
+      <c r="F9" s="48" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" s="17" customFormat="1" ht="38" x14ac:dyDescent="0.2">
+      <c r="A10" s="56" t="s">
+        <v>31</v>
+      </c>
+      <c r="B10" s="38" t="s">
+        <v>32</v>
+      </c>
+      <c r="C10" s="39" t="s">
+        <v>27</v>
+      </c>
+      <c r="D10" s="40" t="s">
+        <v>27</v>
+      </c>
+      <c r="E10" s="41" t="s">
+        <v>33</v>
+      </c>
+      <c r="F10" s="57" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" s="17" customFormat="1" ht="57" x14ac:dyDescent="0.2">
+      <c r="A11" s="50" t="s">
+        <v>41</v>
+      </c>
+      <c r="B11" s="51" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11" s="52" t="s">
+        <v>42</v>
+      </c>
+      <c r="D11" s="53" t="s">
+        <v>26</v>
+      </c>
+      <c r="E11" s="54" t="s">
+        <v>42</v>
+      </c>
+      <c r="F11" s="55" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" s="17" customFormat="1" ht="57" x14ac:dyDescent="0.2">
+      <c r="A12" s="37" t="s">
+        <v>30</v>
+      </c>
+      <c r="B12" s="38" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" s="39" t="s">
+        <v>27</v>
+      </c>
+      <c r="D12" s="40" t="s">
+        <v>27</v>
+      </c>
+      <c r="E12" s="41" t="s">
+        <v>26</v>
+      </c>
+      <c r="F12" s="42" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" s="17" customFormat="1" ht="76" x14ac:dyDescent="0.2">
+      <c r="A13" s="43" t="s">
+        <v>50</v>
+      </c>
+      <c r="B13" s="44" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13" s="45" t="s">
+        <v>27</v>
+      </c>
+      <c r="D13" s="46" t="s">
+        <v>26</v>
+      </c>
+      <c r="E13" s="47" t="s">
+        <v>42</v>
+      </c>
+      <c r="F13" s="48" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" s="17" customFormat="1" ht="38" x14ac:dyDescent="0.2">
+      <c r="A14" s="37" t="s">
+        <v>61</v>
+      </c>
+      <c r="B14" s="38" t="s">
+        <v>26</v>
+      </c>
+      <c r="C14" s="39" t="s">
+        <v>27</v>
+      </c>
+      <c r="D14" s="58" t="s">
+        <v>42</v>
+      </c>
+      <c r="E14" s="41" t="s">
+        <v>26</v>
+      </c>
+      <c r="F14" s="42" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" s="18" customFormat="1" ht="57" x14ac:dyDescent="0.2">
+      <c r="A15" s="59" t="s">
+        <v>36</v>
+      </c>
+      <c r="B15" s="44" t="s">
+        <v>26</v>
+      </c>
+      <c r="C15" s="45" t="s">
+        <v>27</v>
+      </c>
+      <c r="D15" s="46" t="s">
+        <v>27</v>
+      </c>
+      <c r="E15" s="47" t="s">
+        <v>67</v>
+      </c>
+      <c r="F15" s="60" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" s="18" customFormat="1" ht="57" x14ac:dyDescent="0.2">
+      <c r="A16" s="37" t="s">
+        <v>64</v>
+      </c>
+      <c r="B16" s="38" t="s">
+        <v>26</v>
+      </c>
+      <c r="C16" s="39" t="s">
+        <v>27</v>
+      </c>
+      <c r="D16" s="40" t="s">
+        <v>27</v>
+      </c>
+      <c r="E16" s="41" t="s">
+        <v>26</v>
+      </c>
+      <c r="F16" s="42" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" s="18" customFormat="1" ht="38" x14ac:dyDescent="0.2">
+      <c r="A17" s="59" t="s">
+        <v>44</v>
+      </c>
+      <c r="B17" s="44" t="s">
+        <v>26</v>
+      </c>
+      <c r="C17" s="61" t="s">
+        <v>42</v>
+      </c>
+      <c r="D17" s="46" t="s">
+        <v>26</v>
+      </c>
+      <c r="E17" s="47" t="s">
+        <v>26</v>
+      </c>
+      <c r="F17" s="60" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" s="18" customFormat="1" ht="134" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="62" t="s">
+        <v>43</v>
+      </c>
+      <c r="B18" s="63" t="s">
+        <v>45</v>
+      </c>
+      <c r="C18" s="64" t="s">
+        <v>27</v>
+      </c>
+      <c r="D18" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="E18" s="66" t="s">
+        <v>46</v>
+      </c>
+      <c r="F18" s="67" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="19" thickTop="1" x14ac:dyDescent="0.2"/>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B3" r:id="rId1" xr:uid="{978A4675-3171-6E4C-A699-F26B876D2562}"/>
+    <hyperlink ref="C3" r:id="rId2" xr:uid="{B9A34BBA-19FF-F441-B57E-59973E7104DB}"/>
+    <hyperlink ref="D3" r:id="rId3" xr:uid="{B6FCF39D-FA13-1E43-B5EB-36AB35444E04}"/>
+    <hyperlink ref="E3" r:id="rId4" xr:uid="{5FD034E2-35A2-9643-BAAC-F776F2A0A3AB}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
 </file>
</xml_diff>